<commit_message>
Updated Crop Life Cycle and Model Plan
Changed sowing month of Paddy from 1st June to 1st July and Similary
Harvest Month from 1st September to 1st October.
</commit_message>
<xml_diff>
--- a/CropLifeCycle/CropLifeCycle.xlsx
+++ b/CropLifeCycle/CropLifeCycle.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek/code/DataDrivenAgriculture/CropLifeCycle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek\Documents\GitHub\DataDrivenAgriculture\CropLifeCycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="1035" yWindow="1680" windowWidth="27765" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Crop</t>
   </si>
@@ -89,12 +86,6 @@
     <t>31st July</t>
   </si>
   <si>
-    <t>1st June</t>
-  </si>
-  <si>
-    <t>1st September</t>
-  </si>
-  <si>
     <t>31st October</t>
   </si>
   <si>
@@ -144,6 +135,9 @@
   </si>
   <si>
     <t>Paddy/Rice</t>
+  </si>
+  <si>
+    <t>1st July</t>
   </si>
 </sst>
 </file>
@@ -279,6 +273,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -566,17 +563,17 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="18.1640625" customWidth="1"/>
+    <col min="1" max="4" width="18.125" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
@@ -588,7 +585,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -602,16 +599,16 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -634,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -642,22 +639,22 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -665,10 +662,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -680,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -688,22 +685,22 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -711,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -720,36 +717,36 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -757,22 +754,22 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -780,16 +777,16 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
       </c>
       <c r="G10">
         <v>6</v>

</xml_diff>

<commit_message>
Updated Crop Cycle - Wheat Sowing Time
Wheat Sowing time updated to 1st November - 30th November
</commit_message>
<xml_diff>
--- a/CropLifeCycle/CropLifeCycle.xlsx
+++ b/CropLifeCycle/CropLifeCycle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Crop</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>1st November</t>
-  </si>
-  <si>
-    <t>31st December</t>
   </si>
   <si>
     <t>15th April</t>
@@ -563,7 +560,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -599,13 +596,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -642,13 +639,13 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -662,10 +659,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -685,16 +682,16 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -708,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -725,19 +722,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -754,16 +751,16 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
       </c>
       <c r="G9">
         <v>10</v>
@@ -780,13 +777,13 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
       </c>
       <c r="G10">
         <v>6</v>

</xml_diff>

<commit_message>
Yield Prediction - Sugarcane
</commit_message>
<xml_diff>
--- a/CropLifeCycle/CropLifeCycle.xlsx
+++ b/CropLifeCycle/CropLifeCycle.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek\Documents\GitHub\DataDrivenAgriculture\CropLifeCycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek/code/DataDrivenAgriculture/CropLifeCycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1680" windowWidth="27765" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Crop</t>
   </si>
@@ -135,6 +138,9 @@
   </si>
   <si>
     <t>1st July</t>
+  </si>
+  <si>
+    <t>31st December</t>
   </si>
 </sst>
 </file>
@@ -560,12 +566,12 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="18.125" customWidth="1"/>
+    <col min="1" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -582,7 +588,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -605,7 +611,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -628,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -651,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -674,7 +680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -697,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -720,7 +726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -743,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -760,13 +766,13 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Yield Prediction - Wheat
</commit_message>
<xml_diff>
--- a/CropLifeCycle/CropLifeCycle.xlsx
+++ b/CropLifeCycle/CropLifeCycle.xlsx
@@ -566,7 +566,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,7 +792,7 @@
         <v>23</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>